<commit_message>
messing with error bars
</commit_message>
<xml_diff>
--- a/Set-up and Optimization/use as necessary.xlsx
+++ b/Set-up and Optimization/use as necessary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="1460" windowWidth="29300" windowHeight="16300" tabRatio="500" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="2060" yWindow="1460" windowWidth="29300" windowHeight="16300" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="x values" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>X</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>SDOM</t>
+  </si>
+  <si>
+    <t>sqrt</t>
   </si>
 </sst>
 </file>
@@ -99,8 +102,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -191,7 +204,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -234,6 +247,11 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -276,6 +294,11 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3877,7 +3900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4300,15 +4323,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4325,10 +4348,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4349,8 +4375,12 @@
         <f>SQRT(E2)</f>
         <v>3.0550504633038935</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <f t="shared" ref="G2:G66" si="0">_xlfn.STDEV.P(B2:D2)</f>
+        <v>6.8475461947247123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -4364,15 +4394,19 @@
         <v>6</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E66" si="0">AVERAGE(B3:D3)</f>
+        <f t="shared" ref="E3:E66" si="1">AVERAGE(B3:D3)</f>
         <v>7.666666666666667</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="1">SQRT(E3)</f>
+        <f t="shared" ref="F3:F66" si="2">SQRT(E3)</f>
         <v>2.7688746209726918</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1.699673171197595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -4386,15 +4420,19 @@
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.333333333333334</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3665016461206929</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>4.0276819911981905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -4408,15 +4446,19 @@
         <v>13</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.9439202887759488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -4430,15 +4472,19 @@
         <v>21</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.666666666666668</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0662280511902216</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>10.338708279513881</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -4452,15 +4498,19 @@
         <v>24</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.333333333333336</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.110100926607787</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>11.953614051360738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -4474,15 +4524,19 @@
         <v>35</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53.666666666666664</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.32575365861197</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>29.272664533466866</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>0.7</v>
       </c>
@@ -4496,15 +4550,19 @@
         <v>58</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76.666666666666671</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.755950357709132</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>29.272664533466866</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -4518,15 +4576,19 @@
         <v>80</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>96.333333333333329</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.8149545762236379</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>26.712460679532231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -4540,15 +4602,19 @@
         <v>121</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>130.66666666666666</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.430952132988164</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>25.824191930995418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4562,15 +4628,19 @@
         <v>128</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>151.33333333333334</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.301761391497291</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>30.214051182999093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -4584,15 +4654,19 @@
         <v>184</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>198</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.071247279470288</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>31.016124838541646</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -4606,15 +4680,19 @@
         <v>207</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>243.66666666666666</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.609825965290794</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>46.312945154555749</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -4628,15 +4706,19 @@
         <v>265</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279.66666666666669</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.72323732614791</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>44.499687889042796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -4650,15 +4732,19 @@
         <v>293</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>327.66666666666669</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.101565309847285</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>47.618857142476188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -4672,15 +4758,19 @@
         <v>337</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>376</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.390719429665317</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>37.157323190276593</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -4694,15 +4784,19 @@
         <v>407</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>404.33333333333331</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.108041509140897</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>18.873850222522755</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -4716,15 +4810,19 @@
         <v>449</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>475.66666666666669</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.80978373727412</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>19.955506062794353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -4738,15 +4836,19 @@
         <v>547</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>551.66666666666663</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23.48758537327042</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>32.826141344293809</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -4760,15 +4862,19 @@
         <v>571</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>589</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.269322199023193</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>17.107503227141788</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4782,15 +4888,19 @@
         <v>639</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>665.66666666666663</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.800516790689805</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>50.215092905973549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -4804,15 +4914,19 @@
         <v>727</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>762</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27.604347483684521</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>41.960298696108765</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -4826,15 +4940,19 @@
         <v>718</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>779.33333333333337</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27.916542288280141</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>64.819407244709936</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -4848,15 +4966,19 @@
         <v>945</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>874</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.563490998188964</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>54.668699149208464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -4870,15 +4992,19 @@
         <v>897</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>926.33333333333337</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.43572462310259</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>38.002923864121584</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -4892,15 +5018,19 @@
         <v>1032</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1040</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.249030993194197</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>25.13961017995307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -4914,15 +5044,19 @@
         <v>984</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1038.6666666666667</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.22835190739152</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>42.975445185464785</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -4936,15 +5070,19 @@
         <v>1059</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1120.3333333333333</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.471380810079125</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>66.659999666633325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -4958,15 +5096,19 @@
         <v>1121</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1160</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.058772731852805</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>41.206795556073033</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -4980,15 +5122,19 @@
         <v>1231</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1171</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.219877264537345</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>42.457822208241751</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>3</v>
       </c>
@@ -5002,15 +5148,19 @@
         <v>1268</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1232.6666666666667</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.109352979892222</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>26.836956277160461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -5024,15 +5174,19 @@
         <v>1241</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1238</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.185224171518364</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -5046,15 +5200,19 @@
         <v>1284</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1277.6666666666667</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.74446344074375</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>14.197026292697903</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -5068,15 +5226,19 @@
         <v>1246</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1285.3333333333333</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.851545759330008</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>30.390056853443951</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -5090,15 +5252,19 @@
         <v>1219</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1258</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.468295701936398</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>28.437065014988214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -5112,15 +5278,19 @@
         <v>1306</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1281.3333333333333</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.795716689756794</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>20.853989759489405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>3.6</v>
       </c>
@@ -5134,15 +5304,19 @@
         <v>1238</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1281.3333333333333</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.795716689756794</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>48.472214262972926</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>3.7</v>
       </c>
@@ -5156,15 +5330,19 @@
         <v>1286</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1252</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.383612025908263</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>41.880783182743848</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>3.8</v>
       </c>
@@ -5178,15 +5356,19 @@
         <v>1211</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1214.3333333333333</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.847285881877994</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>14.079141387961918</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>3.9</v>
       </c>
@@ -5200,15 +5382,19 @@
         <v>1197</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1240.6666666666667</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.223098481914775</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>63.88705311372216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>4</v>
       </c>
@@ -5222,15 +5408,19 @@
         <v>1196</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1157.6666666666667</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.024500976012369</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>29.578520735305357</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>4.0999999999999996</v>
       </c>
@@ -5244,15 +5434,19 @@
         <v>1098</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1114</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.376638536557273</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>13.063945294843617</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>4.2</v>
       </c>
@@ -5266,15 +5460,19 @@
         <v>1106</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1096.3333333333333</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.110924682547498</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>25.037749277618563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>4.3</v>
       </c>
@@ -5288,15 +5486,19 @@
         <v>1039</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>998.66666666666663</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.60168771864355</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>34.836124290103733</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>4.4000000000000004</v>
       </c>
@@ -5310,15 +5512,19 @@
         <v>929</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>948</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.789608636681304</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>23.423634787681152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>4.5</v>
       </c>
@@ -5332,15 +5538,19 @@
         <v>944</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>914.33333333333337</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.23794525647094</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>39.160637833870318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>4.5999999999999996</v>
       </c>
@@ -5354,15 +5564,19 @@
         <v>896</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>870</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.49576240750525</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>18.384776310850235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>4.7</v>
       </c>
@@ -5376,15 +5590,19 @@
         <v>827</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>804.33333333333337</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.360771028541048</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>20.677416559027762</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>4.8</v>
       </c>
@@ -5398,15 +5616,19 @@
         <v>704</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>705.66666666666663</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26.564387187862373</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>5.4365021434333638</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>4.9000000000000004</v>
       </c>
@@ -5420,15 +5642,19 @@
         <v>642</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>661</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.709920264364882</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>16.872067646458351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>5</v>
       </c>
@@ -5442,15 +5668,19 @@
         <v>577</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>592</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.331050121192877</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>12.675435561221029</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>5.0999999999999996</v>
       </c>
@@ -5464,15 +5694,19 @@
         <v>472</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>492</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22.181073012818835</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>21.602468994692867</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>5.2</v>
       </c>
@@ -5486,15 +5720,19 @@
         <v>411</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>449.33333333333331</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.197484127446195</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>27.980151695244412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>5.3</v>
       </c>
@@ -5508,15 +5746,19 @@
         <v>401</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>371</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.261360284258224</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>26.770630673681683</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>5.4</v>
       </c>
@@ -5530,15 +5772,19 @@
         <v>369</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>343.66666666666669</v>
       </c>
       <c r="F56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.538248748645778</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>18.080068829760823</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>5.5</v>
       </c>
@@ -5552,15 +5798,19 @@
         <v>342</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
       <c r="F57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.146428199482248</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>33.950945004029961</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>5.6</v>
       </c>
@@ -5574,15 +5824,19 @@
         <v>274</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>256.33333333333331</v>
       </c>
       <c r="F58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.010413278030438</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>14.290634073484011</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>5.7</v>
       </c>
@@ -5596,15 +5850,19 @@
         <v>219</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>198.33333333333334</v>
       </c>
       <c r="F59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.083086782851739</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>15.173075568988057</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>5.8</v>
       </c>
@@ -5618,15 +5876,19 @@
         <v>162</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>157.33333333333334</v>
       </c>
       <c r="F60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.54325848148452</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>17.46106780494506</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>5.9</v>
       </c>
@@ -5640,15 +5902,19 @@
         <v>151</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>138.66666666666666</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.775681155103795</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>10.208928554075703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>6</v>
       </c>
@@ -5662,15 +5928,19 @@
         <v>139</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110.33333333333333</v>
       </c>
       <c r="F62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.503967504392486</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>20.853989759489405</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>6.1</v>
       </c>
@@ -5684,15 +5954,19 @@
         <v>92</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76.666666666666671</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.755950357709132</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>11.115554667022044</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>6.2</v>
       </c>
@@ -5706,15 +5980,19 @@
         <v>69</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2111025509279782</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>14.30617582258329</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>6.3</v>
       </c>
@@ -5728,15 +6006,19 @@
         <v>55</v>
       </c>
       <c r="E65" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42.666666666666664</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5319726474218083</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>9.1772665986241364</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>6.4</v>
       </c>
@@ -5750,15 +6032,19 @@
         <v>37</v>
       </c>
       <c r="E66" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0990195135927845</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>8.0415587212098796</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>6.5</v>
       </c>
@@ -5772,15 +6058,19 @@
         <v>21</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E82" si="2">AVERAGE(B67:D67)</f>
+        <f t="shared" ref="E67:E82" si="3">AVERAGE(B67:D67)</f>
         <v>17.333333333333332</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F82" si="3">SQRT(E67)</f>
+        <f t="shared" ref="F67:F82" si="4">SQRT(E67)</f>
         <v>4.1633319989322652</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <f t="shared" ref="G67:G82" si="5">_xlfn.STDEV.P(B67:D67)</f>
+        <v>3.858612300930075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>6.6</v>
       </c>
@@ -5794,15 +6084,19 @@
         <v>21</v>
       </c>
       <c r="E68" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="F68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.6055512754639891</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <f t="shared" si="5"/>
+        <v>5.8878405775518976</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>6.7</v>
       </c>
@@ -5816,15 +6110,19 @@
         <v>7</v>
       </c>
       <c r="E69" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.666666666666667</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7688746209726918</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <f t="shared" si="5"/>
+        <v>1.699673171197595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>6.8</v>
       </c>
@@ -5838,15 +6136,19 @@
         <v>3</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2360679774997898</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <f t="shared" si="5"/>
+        <v>2.1602468994692869</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>6.9</v>
       </c>
@@ -5860,15 +6162,19 @@
         <v>5</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.333333333333333</v>
       </c>
       <c r="F71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.70801280154532</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <f t="shared" si="5"/>
+        <v>1.699673171197595</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>7</v>
       </c>
@@ -5882,15 +6188,19 @@
         <v>9</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0550504633038935</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <f t="shared" si="5"/>
+        <v>4.4969125210773466</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>7.1</v>
       </c>
@@ -5904,15 +6214,19 @@
         <v>15</v>
       </c>
       <c r="E73" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="F73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.872983346207417</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <f t="shared" si="5"/>
+        <v>1.6329931618554521</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>7.2</v>
       </c>
@@ -5926,15 +6240,19 @@
         <v>19</v>
       </c>
       <c r="E74" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="F74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.872983346207417</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <f t="shared" si="5"/>
+        <v>2.9439202887759488</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>7.3</v>
       </c>
@@ -5948,15 +6266,19 @@
         <v>20</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="F75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.8989794855663558</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>5.6568542494923806</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>7.4</v>
       </c>
@@ -5970,15 +6292,19 @@
         <v>20</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25.333333333333332</v>
       </c>
       <c r="F76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.0332229568471663</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>5.5577773335110221</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>7.5</v>
       </c>
@@ -5992,15 +6318,19 @@
         <v>34</v>
       </c>
       <c r="E77" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34.333333333333336</v>
       </c>
       <c r="F77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8594652770823155</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <f t="shared" si="5"/>
+        <v>1.247219128924647</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>7.6</v>
       </c>
@@ -6014,15 +6344,19 @@
         <v>35</v>
       </c>
       <c r="E78" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.666666666666664</v>
       </c>
       <c r="F78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.1373175465073224</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <f t="shared" si="5"/>
+        <v>2.0548046676563256</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>7.7</v>
       </c>
@@ -6036,15 +6370,19 @@
         <v>41</v>
       </c>
       <c r="E79" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40.333333333333336</v>
       </c>
       <c r="F79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.3508529610858835</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>0.47140452079103168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>7.8</v>
       </c>
@@ -6058,15 +6396,19 @@
         <v>53</v>
       </c>
       <c r="E80" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39.666666666666664</v>
       </c>
       <c r="F80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.2981478758970608</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <f t="shared" si="5"/>
+        <v>9.5684667296048822</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>7.9</v>
       </c>
@@ -6080,15 +6422,19 @@
         <v>32</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="F81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.1231056256176606</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <f t="shared" si="5"/>
+        <v>10.801234497346433</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>8</v>
       </c>
@@ -6102,12 +6448,16 @@
         <v>15</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0550504633038935</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="5"/>
+        <v>4.4969125210773466</v>
       </c>
     </row>
   </sheetData>
@@ -6126,15 +6476,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6151,10 +6501,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6175,8 +6528,12 @@
         <f>SQRT(E2)</f>
         <v>7.3029674334022152</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <f>_xlfn.STDEV.P(B2:D2)</f>
+        <v>8.055363982396381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -6197,8 +6554,12 @@
         <f t="shared" ref="F3:F66" si="1">SQRT(E3)</f>
         <v>6.831300510639732</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="2">_xlfn.STDEV.P(B3:D3)</f>
+        <v>4.0276819911981914</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -6219,8 +6580,12 @@
         <f t="shared" si="1"/>
         <v>7.1180521680208741</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>9.8432153734889329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -6241,8 +6606,12 @@
         <f t="shared" si="1"/>
         <v>6.7823299831252681</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>6.3770421565696633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -6263,8 +6632,12 @@
         <f t="shared" si="1"/>
         <v>6.5064070986477116</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>3.6817870057290873</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -6285,8 +6658,12 @@
         <f t="shared" si="1"/>
         <v>6.4549722436790278</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>2.0548046676563256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -6307,8 +6684,12 @@
         <f t="shared" si="1"/>
         <v>5.5677643628300215</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>9.41629792788369</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>0.7</v>
       </c>
@@ -6329,8 +6710,12 @@
         <f t="shared" si="1"/>
         <v>5.8022983951764031</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>2.8674417556808756</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -6351,8 +6736,12 @@
         <f t="shared" si="1"/>
         <v>4.7609522856952333</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>4.9888765156985881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -6373,8 +6762,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>4.3204937989385739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -6395,8 +6788,12 @@
         <f t="shared" si="1"/>
         <v>3.7416573867739413</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -6417,8 +6814,12 @@
         <f t="shared" si="1"/>
         <v>3.3166247903553998</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0.81649658092772603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -6439,8 +6840,12 @@
         <f t="shared" si="1"/>
         <v>2.6457513110645907</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1.6329931618554521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -6461,8 +6866,12 @@
         <f t="shared" si="1"/>
         <v>2.8284271247461903</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -6483,8 +6892,12 @@
         <f t="shared" si="1"/>
         <v>2.8867513459481291</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>3.2998316455372216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -6505,8 +6918,12 @@
         <f t="shared" si="1"/>
         <v>4.1633319989322652</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>3.2998316455372216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -6527,8 +6944,12 @@
         <f t="shared" si="1"/>
         <v>4.8304589153964796</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>6.6499791144200007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -6549,8 +6970,12 @@
         <f t="shared" si="1"/>
         <v>5.7445626465380286</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>5.0990195135927845</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -6571,8 +6996,12 @@
         <f t="shared" si="1"/>
         <v>6.7082039324993694</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>8.1649658092772608</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -6593,8 +7022,12 @@
         <f t="shared" si="1"/>
         <v>7.9791394690572153</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>1.247219128924647</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>2</v>
       </c>
@@ -6615,8 +7048,12 @@
         <f t="shared" si="1"/>
         <v>9.3452305125841235</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>10.338708279513881</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -6637,8 +7074,12 @@
         <f t="shared" si="1"/>
         <v>10.392304845413264</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>12.192894105447921</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -6659,8 +7100,12 @@
         <f t="shared" si="1"/>
         <v>12.151817422372122</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>14.055445761538676</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -6681,8 +7126,12 @@
         <f t="shared" si="1"/>
         <v>13.45362404707371</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>15.748015748023622</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -6703,8 +7152,12 @@
         <f t="shared" si="1"/>
         <v>14.866068747318506</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>5.8878405775518976</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -6725,8 +7178,12 @@
         <f t="shared" si="1"/>
         <v>16.532795690182994</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>19.344824171395878</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -6747,8 +7204,12 @@
         <f t="shared" si="1"/>
         <v>17.710637105046974</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>2.4944382578492941</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -6769,8 +7230,12 @@
         <f t="shared" si="1"/>
         <v>19.209372712298546</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>15.297058540778355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -6791,8 +7256,12 @@
         <f t="shared" si="1"/>
         <v>20.728402414722336</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>26.599916457680006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -6813,8 +7282,12 @@
         <f t="shared" si="1"/>
         <v>21.679483388678801</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>5.0990195135927845</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>3</v>
       </c>
@@ -6835,8 +7308,12 @@
         <f t="shared" si="1"/>
         <v>23.330952259462823</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>26.948510575210314</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -6857,8 +7334,12 @@
         <f t="shared" si="1"/>
         <v>24.372115213907882</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>20.992061991778385</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -6879,8 +7360,12 @@
         <f t="shared" si="1"/>
         <v>26.121510931286753</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>10.656244908763854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -6901,8 +7386,12 @@
         <f t="shared" si="1"/>
         <v>27.055498516937366</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>31.016124838541646</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -6923,8 +7412,12 @@
         <f t="shared" si="1"/>
         <v>27.300793639257694</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>23.442601296689656</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -6945,8 +7438,12 @@
         <f t="shared" si="1"/>
         <v>29.03446228191595</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>7.7888809636986149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>3.6</v>
       </c>
@@ -6967,8 +7464,12 @@
         <f t="shared" si="1"/>
         <v>29.597297173897484</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>31.15552385479446</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>3.7</v>
       </c>
@@ -6989,8 +7490,12 @@
         <f t="shared" si="1"/>
         <v>30.924639582917266</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>19.48218559493661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>3.8</v>
       </c>
@@ -7011,8 +7516,12 @@
         <f t="shared" si="1"/>
         <v>31.911335499056339</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>23.170862929310353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>3.9</v>
       </c>
@@ -7033,8 +7542,12 @@
         <f t="shared" si="1"/>
         <v>31.927000067863148</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>12.391753530294071</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>4</v>
       </c>
@@ -7055,8 +7568,12 @@
         <f t="shared" si="1"/>
         <v>33.020195840323737</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>12.36482466066094</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>4.0999999999999996</v>
       </c>
@@ -7077,8 +7594,12 @@
         <f t="shared" si="1"/>
         <v>32.787192621510002</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>9.8994949366116654</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>4.2</v>
       </c>
@@ -7099,8 +7620,12 @@
         <f t="shared" si="1"/>
         <v>33.630343441600473</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>30.430248109405877</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>4.3</v>
       </c>
@@ -7121,8 +7646,12 @@
         <f t="shared" si="1"/>
         <v>33.773757070640912</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>12.364824660660938</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>4.4000000000000004</v>
       </c>
@@ -7143,8 +7672,12 @@
         <f t="shared" si="1"/>
         <v>33.788558221188822</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>19.601587237318874</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>4.5</v>
       </c>
@@ -7165,8 +7698,12 @@
         <f t="shared" si="1"/>
         <v>33.837848631377263</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>9.0921211313239034</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>4.5999999999999996</v>
       </c>
@@ -7187,8 +7724,12 @@
         <f t="shared" si="1"/>
         <v>33.660065359413672</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>32.629230249374054</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>4.7</v>
       </c>
@@ -7209,8 +7750,12 @@
         <f t="shared" si="1"/>
         <v>33.803352890899248</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>20.499322482029065</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>4.8</v>
       </c>
@@ -7231,8 +7776,12 @@
         <f t="shared" si="1"/>
         <v>33.371644650311538</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>39.668067202165972</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>4.9000000000000004</v>
       </c>
@@ -7253,8 +7802,12 @@
         <f t="shared" si="1"/>
         <v>32.924155266308659</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>35.014282800023196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>5</v>
       </c>
@@ -7275,8 +7828,12 @@
         <f t="shared" si="1"/>
         <v>32.161053050752756</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>9.0308114560960444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>5.0999999999999996</v>
       </c>
@@ -7297,8 +7854,12 @@
         <f t="shared" si="1"/>
         <v>31.900888179902871</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <f t="shared" si="2"/>
+        <v>9.0308114560960444</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>5.2</v>
       </c>
@@ -7319,8 +7880,12 @@
         <f t="shared" si="1"/>
         <v>31.759513010540111</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <f t="shared" si="2"/>
+        <v>28.859814429217813</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>5.3</v>
       </c>
@@ -7341,8 +7906,12 @@
         <f t="shared" si="1"/>
         <v>30.441200151548998</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <f t="shared" si="2"/>
+        <v>16.659998666133067</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>5.4</v>
       </c>
@@ -7363,8 +7932,12 @@
         <f t="shared" si="1"/>
         <v>29.507061301774304</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <f t="shared" si="2"/>
+        <v>4.6427960923947067</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>5.5</v>
       </c>
@@ -7385,8 +7958,12 @@
         <f t="shared" si="1"/>
         <v>28.687976575562104</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <f t="shared" si="2"/>
+        <v>36.120169803956721</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>5.6</v>
       </c>
@@ -7407,8 +7984,12 @@
         <f t="shared" si="1"/>
         <v>27.386127875258307</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>15.297058540778355</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>5.7</v>
       </c>
@@ -7429,8 +8010,12 @@
         <f t="shared" si="1"/>
         <v>26.851443164195103</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <f t="shared" si="2"/>
+        <v>17.048949136725895</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>5.8</v>
       </c>
@@ -7451,8 +8036,12 @@
         <f t="shared" si="1"/>
         <v>25.219040425836983</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <f t="shared" si="2"/>
+        <v>19.442222095223581</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>5.9</v>
       </c>
@@ -7473,8 +8062,12 @@
         <f t="shared" si="1"/>
         <v>23.881652650797292</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>37.615008824788127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>6</v>
       </c>
@@ -7495,8 +8088,12 @@
         <f t="shared" si="1"/>
         <v>22.300971578236975</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <f t="shared" si="2"/>
+        <v>35.367907612536101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>6.1</v>
       </c>
@@ -7517,8 +8114,12 @@
         <f t="shared" si="1"/>
         <v>21.756225162774292</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <f t="shared" si="2"/>
+        <v>15.965240019770729</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>6.2</v>
       </c>
@@ -7539,8 +8140,12 @@
         <f t="shared" si="1"/>
         <v>20.083160441856091</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <f t="shared" si="2"/>
+        <v>7.4087035902976224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>6.3</v>
       </c>
@@ -7561,8 +8166,12 @@
         <f t="shared" si="1"/>
         <v>18.574175621006709</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <f t="shared" si="2"/>
+        <v>15.57776192739723</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>6.4</v>
       </c>
@@ -7583,8 +8192,12 @@
         <f t="shared" si="1"/>
         <v>17.530925056406275</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <f t="shared" si="2"/>
+        <v>10.143416036468626</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>6.5</v>
       </c>
@@ -7598,15 +8211,19 @@
         <v>240</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E82" si="2">AVERAGE(B67:D67)</f>
+        <f t="shared" ref="E67:E82" si="3">AVERAGE(B67:D67)</f>
         <v>252.33333333333334</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F82" si="3">SQRT(E67)</f>
+        <f t="shared" ref="F67:F82" si="4">SQRT(E67)</f>
         <v>15.88500340992514</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <f t="shared" ref="G67:G82" si="5">_xlfn.STDEV.P(B67:D67)</f>
+        <v>10.656244908763853</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>6.6</v>
       </c>
@@ -7620,15 +8237,19 @@
         <v>201</v>
       </c>
       <c r="E68" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>202.33333333333334</v>
       </c>
       <c r="F68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.224392195567912</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <f t="shared" si="5"/>
+        <v>7.4087035902976224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>6.7</v>
       </c>
@@ -7642,15 +8263,19 @@
         <v>170</v>
       </c>
       <c r="E69" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>156.33333333333334</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.503332889007368</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <f t="shared" si="5"/>
+        <v>14.055445761538676</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>6.8</v>
       </c>
@@ -7664,15 +8289,19 @@
         <v>119</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125.66666666666667</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.210114480533491</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <f t="shared" si="5"/>
+        <v>8.0553639823963827</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>6.9</v>
       </c>
@@ -7686,15 +8315,19 @@
         <v>107</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106.33333333333333</v>
       </c>
       <c r="F71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.311805532172013</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <f t="shared" si="5"/>
+        <v>1.699673171197595</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>7</v>
       </c>
@@ -7708,15 +8341,19 @@
         <v>73</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76.666666666666671</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.755950357709132</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <f t="shared" si="5"/>
+        <v>10.530379332620877</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>7.1</v>
       </c>
@@ -7730,15 +8367,19 @@
         <v>44</v>
       </c>
       <c r="E73" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.666666666666664</v>
       </c>
       <c r="F73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.047458170621991</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <f t="shared" si="5"/>
+        <v>4.4969125210773475</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>7.2</v>
       </c>
@@ -7752,15 +8393,19 @@
         <v>44</v>
       </c>
       <c r="E74" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="F74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.4031242374328485</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <f t="shared" si="5"/>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>7.3</v>
       </c>
@@ -7774,15 +8419,19 @@
         <v>25</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="F75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.0990195135927845</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>5.3541261347363367</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>7.4</v>
       </c>
@@ -7796,15 +8445,19 @@
         <v>13</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="F76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.6055512754639891</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>3.2659863237109041</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>7.5</v>
       </c>
@@ -7818,15 +8471,19 @@
         <v>8</v>
       </c>
       <c r="E77" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.6666666666666661</v>
       </c>
       <c r="F77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9439202887759488</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <f t="shared" si="5"/>
+        <v>3.2998316455372216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>7.6</v>
       </c>
@@ -7840,15 +8497,19 @@
         <v>7</v>
       </c>
       <c r="E78" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.333333333333333</v>
       </c>
       <c r="F78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.70801280154532</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <f t="shared" si="5"/>
+        <v>0.47140452079103168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>7.7</v>
       </c>
@@ -7862,15 +8523,19 @@
         <v>6</v>
       </c>
       <c r="E79" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="F79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>5.715476066494082</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>7.8</v>
       </c>
@@ -7884,15 +8549,19 @@
         <v>6</v>
       </c>
       <c r="E80" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.333333333333333</v>
       </c>
       <c r="F80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3094010767585029</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <f t="shared" si="5"/>
+        <v>0.94280904158206336</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>7.9</v>
       </c>
@@ -7906,15 +8575,19 @@
         <v>1</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2360679774997898</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <f t="shared" si="5"/>
+        <v>2.9439202887759488</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>8</v>
       </c>
@@ -7928,12 +8601,16 @@
         <v>5</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.666666666666667</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1602468994692869</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="5"/>
+        <v>2.0548046676563256</v>
       </c>
     </row>
   </sheetData>
@@ -7949,15 +8626,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="I13" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7974,10 +8651,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7998,8 +8678,12 @@
         <f>SQRT(E2)</f>
         <v>7.8951461882180078</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <f>_xlfn.STDEV.P(B2:D2)</f>
+        <v>7.1336448530108987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -8020,8 +8704,12 @@
         <f t="shared" ref="F3:F66" si="1">SQRT(E3)</f>
         <v>7.32575365861197</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="2">_xlfn.STDEV.P(B3:D3)</f>
+        <v>4.6427960923947067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -8042,8 +8730,12 @@
         <f t="shared" si="1"/>
         <v>8.0208062770106423</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>13.816254517375137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -8064,8 +8756,12 @@
         <f t="shared" si="1"/>
         <v>9.0369611411506394</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>8.1785627642568652</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -8086,8 +8782,12 @@
         <f t="shared" si="1"/>
         <v>6.7082039324993694</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>7.8740078740118111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -8108,8 +8808,12 @@
         <f t="shared" si="1"/>
         <v>3.9157800414902435</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>4.4969125210773466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -8130,8 +8834,12 @@
         <f t="shared" si="1"/>
         <v>5.3851648071345037</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>9.8994949366116654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>0.7</v>
       </c>
@@ -8152,8 +8860,12 @@
         <f t="shared" si="1"/>
         <v>9.1833182093039412</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>10.873004286866728</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -8174,8 +8886,12 @@
         <f t="shared" si="1"/>
         <v>12.436505404118419</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>13.123346456686352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -8196,8 +8912,12 @@
         <f t="shared" si="1"/>
         <v>13.165611772087667</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>1.247219128924647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -8218,8 +8938,12 @@
         <f t="shared" si="1"/>
         <v>13.4412301024373</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>14.636332266733433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -8240,8 +8964,12 @@
         <f t="shared" si="1"/>
         <v>13.4412301024373</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>5.4365021434333629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -8262,8 +8990,12 @@
         <f t="shared" si="1"/>
         <v>14.282856857085701</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>7.7888809636986149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -8284,8 +9016,12 @@
         <f t="shared" si="1"/>
         <v>16.552945357246848</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>14.165686240583852</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -8306,8 +9042,12 @@
         <f t="shared" si="1"/>
         <v>16.663332999933317</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>8.4983658559879736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -8328,8 +9068,12 @@
         <f t="shared" si="1"/>
         <v>16.921386861996073</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>27.980151695244412</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -8350,8 +9094,12 @@
         <f t="shared" si="1"/>
         <v>17.925772879665004</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>15.326085243430198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -8372,8 +9120,12 @@
         <f t="shared" si="1"/>
         <v>22.375581929117882</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>21.913973218524799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -8394,8 +9146,12 @@
         <f t="shared" si="1"/>
         <v>27.934447074057747</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>6.128258770283411</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -8416,8 +9172,12 @@
         <f t="shared" si="1"/>
         <v>32.03123475609393</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>25.80697580112788</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>2</v>
       </c>
@@ -8438,8 +9198,12 @@
         <f t="shared" si="1"/>
         <v>31.203632267200348</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>24.417662095749915</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -8460,8 +9224,12 @@
         <f t="shared" si="1"/>
         <v>25.534290669607408</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>40.718546143004666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -8482,8 +9250,12 @@
         <f t="shared" si="1"/>
         <v>18.850287354131588</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>5.4365021434333638</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -8504,8 +9276,12 @@
         <f t="shared" si="1"/>
         <v>21.908902300206645</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>12.027745701779143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -8526,8 +9302,12 @@
         <f t="shared" si="1"/>
         <v>33.171272711991818</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>39.194670839569781</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -8548,8 +9328,12 @@
         <f t="shared" si="1"/>
         <v>45.258516693914459</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>12.256517540566822</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -8570,8 +9354,12 @@
         <f t="shared" si="1"/>
         <v>49.267974723275699</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>58.151144060590553</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -8592,8 +9380,12 @@
         <f t="shared" si="1"/>
         <v>44.944410108488462</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>72.221880341071156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -8614,8 +9406,12 @@
         <f t="shared" si="1"/>
         <v>32.083225108042569</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>10.077477638553981</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -8636,8 +9432,12 @@
         <f t="shared" si="1"/>
         <v>17.897858344878397</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>3.0912061651652349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>3</v>
       </c>
@@ -8658,8 +9458,12 @@
         <f t="shared" si="1"/>
         <v>25.599479161368368</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>27.620443314488796</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -8680,8 +9484,12 @@
         <f t="shared" si="1"/>
         <v>44.91844461539899</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>55.571775410024671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -8702,8 +9510,12 @@
         <f t="shared" si="1"/>
         <v>57.75523064335097</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>110.57827795528178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -8724,8 +9536,12 @@
         <f t="shared" si="1"/>
         <v>61.489836558572833</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>14.352700094407323</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -8746,8 +9562,12 @@
         <f t="shared" si="1"/>
         <v>52.494444150468595</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>55.643707840349954</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -8768,8 +9588,12 @@
         <f t="shared" si="1"/>
         <v>34.942810419312295</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>90.136932866981155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>3.6</v>
       </c>
@@ -8790,8 +9614,12 @@
         <f t="shared" si="1"/>
         <v>15.110702608857515</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>10.780641085864152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>3.7</v>
       </c>
@@ -8812,8 +9640,12 @@
         <f t="shared" si="1"/>
         <v>28.189832682487964</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>21.561282171728305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>3.8</v>
       </c>
@@ -8834,8 +9666,12 @@
         <f t="shared" si="1"/>
         <v>49.863146043278633</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>20.417857108151406</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>3.9</v>
       </c>
@@ -8856,8 +9692,12 @@
         <f t="shared" si="1"/>
         <v>63.718129288295962</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>71.721684308164427</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>4</v>
       </c>
@@ -8878,8 +9718,12 @@
         <f t="shared" si="1"/>
         <v>65.386033167132354</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>123.92560492309713</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>4.0999999999999996</v>
       </c>
@@ -8900,8 +9744,12 @@
         <f t="shared" si="1"/>
         <v>53.322915649215332</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>42.757715353164301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>4.2</v>
       </c>
@@ -8922,8 +9770,12 @@
         <f t="shared" si="1"/>
         <v>33.316662497915367</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>13.4412301024373</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>4.3</v>
       </c>
@@ -8944,8 +9796,12 @@
         <f t="shared" si="1"/>
         <v>13.45362404707371</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>8.6409875978771478</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>4.4000000000000004</v>
       </c>
@@ -8966,8 +9822,12 @@
         <f t="shared" si="1"/>
         <v>28.583211855912904</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>17.907168024751059</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>4.5</v>
       </c>
@@ -8988,8 +9848,12 @@
         <f t="shared" si="1"/>
         <v>49.863146043278633</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>32.96799795087486</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>4.5999999999999996</v>
       </c>
@@ -9010,8 +9874,12 @@
         <f t="shared" si="1"/>
         <v>60.296489671179586</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>33.8066397160216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>4.7</v>
       </c>
@@ -9032,8 +9900,12 @@
         <f t="shared" si="1"/>
         <v>59.483891376853727</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>64.251242962469007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>4.8</v>
       </c>
@@ -9054,8 +9926,12 @@
         <f t="shared" si="1"/>
         <v>46.925472826600263</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>69.531767320172918</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>4.9000000000000004</v>
       </c>
@@ -9076,8 +9952,12 @@
         <f t="shared" si="1"/>
         <v>27.682726262659415</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>9.3926685357369148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>5</v>
       </c>
@@ -9098,8 +9978,12 @@
         <f t="shared" si="1"/>
         <v>14.387494569938159</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>6.6833125519211407</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>5.0999999999999996</v>
       </c>
@@ -9120,8 +10004,12 @@
         <f t="shared" si="1"/>
         <v>27.646579052991953</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <f t="shared" si="2"/>
+        <v>43.37690117511341</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>5.2</v>
       </c>
@@ -9142,8 +10030,12 @@
         <f t="shared" si="1"/>
         <v>42.217689815210555</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <f t="shared" si="2"/>
+        <v>33.068951533962419</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>5.3</v>
       </c>
@@ -9164,8 +10056,12 @@
         <f t="shared" si="1"/>
         <v>48.531776531807836</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <f t="shared" si="2"/>
+        <v>54.322084725173141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>5.4</v>
       </c>
@@ -9186,8 +10082,12 @@
         <f t="shared" si="1"/>
         <v>45.70193285482209</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <f t="shared" si="2"/>
+        <v>18.445113776342563</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>5.5</v>
       </c>
@@ -9208,8 +10108,12 @@
         <f t="shared" si="1"/>
         <v>35.142566781611158</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <f t="shared" si="2"/>
+        <v>54.485472069778993</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>5.6</v>
       </c>
@@ -9230,8 +10134,12 @@
         <f t="shared" si="1"/>
         <v>21.817424229271428</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>10.033277962194941</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>5.7</v>
       </c>
@@ -9252,8 +10160,12 @@
         <f t="shared" si="1"/>
         <v>15.264337522473747</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <f t="shared" si="2"/>
+        <v>15.748015748023622</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>5.8</v>
       </c>
@@ -9274,8 +10186,12 @@
         <f t="shared" si="1"/>
         <v>22.649503305812249</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <f t="shared" si="2"/>
+        <v>7.1180521680208741</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>5.9</v>
       </c>
@@ -9296,8 +10212,12 @@
         <f t="shared" si="1"/>
         <v>28.821288428289716</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>24.143091949642425</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>6</v>
       </c>
@@ -9318,8 +10238,12 @@
         <f t="shared" si="1"/>
         <v>31.091263510296049</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <f t="shared" si="2"/>
+        <v>37.606146069787876</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>6.1</v>
       </c>
@@ -9340,8 +10264,12 @@
         <f t="shared" si="1"/>
         <v>27.54995462791182</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <f t="shared" si="2"/>
+        <v>8.2865352631040352</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>6.2</v>
       </c>
@@ -9362,8 +10290,12 @@
         <f t="shared" si="1"/>
         <v>21.047565179849187</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <f t="shared" si="2"/>
+        <v>10.677078252031311</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>6.3</v>
       </c>
@@ -9384,8 +10316,12 @@
         <f t="shared" si="1"/>
         <v>15.758595538097085</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <f t="shared" si="2"/>
+        <v>13.67073110293992</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>6.4</v>
       </c>
@@ -9406,8 +10342,12 @@
         <f t="shared" si="1"/>
         <v>14.059397805975427</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <f t="shared" si="2"/>
+        <v>3.2998316455372221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>6.5</v>
       </c>
@@ -9421,15 +10361,19 @@
         <v>248</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E82" si="2">AVERAGE(B67:D67)</f>
+        <f t="shared" ref="E67:E82" si="3">AVERAGE(B67:D67)</f>
         <v>224.33333333333334</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F82" si="3">SQRT(E67)</f>
+        <f t="shared" ref="F67:F82" si="4">SQRT(E67)</f>
         <v>14.977761292440647</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <f t="shared" ref="G67:G82" si="5">_xlfn.STDEV.P(B67:D67)</f>
+        <v>17.133463034528528</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>6.6</v>
       </c>
@@ -9443,15 +10387,19 @@
         <v>233</v>
       </c>
       <c r="E68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>229</v>
       </c>
       <c r="F68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.132745950421556</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <f t="shared" si="5"/>
+        <v>2.9439202887759488</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>6.7</v>
       </c>
@@ -9465,15 +10413,19 @@
         <v>184</v>
       </c>
       <c r="E69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>187.66666666666666</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.699148392023011</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <f t="shared" si="5"/>
+        <v>3.2998316455372221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>6.8</v>
       </c>
@@ -9487,15 +10439,19 @@
         <v>143</v>
       </c>
       <c r="E70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130.66666666666666</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.430952132988164</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <f t="shared" si="5"/>
+        <v>10.656244908763853</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>6.9</v>
       </c>
@@ -9509,15 +10465,19 @@
         <v>125</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>127.33333333333333</v>
       </c>
       <c r="F71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.284207253207171</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <f t="shared" si="5"/>
+        <v>16.006942938057293</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>7</v>
       </c>
@@ -9531,15 +10491,19 @@
         <v>135</v>
       </c>
       <c r="E72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.445523142259598</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <f t="shared" si="5"/>
+        <v>11.775681155103795</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>7.1</v>
       </c>
@@ -9553,15 +10517,19 @@
         <v>106</v>
       </c>
       <c r="E73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.33333333333333</v>
       </c>
       <c r="F73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.263202878893768</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <f t="shared" si="5"/>
+        <v>5.7348835113617511</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>7.2</v>
       </c>
@@ -9575,15 +10543,19 @@
         <v>81</v>
       </c>
       <c r="E74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72.666666666666671</v>
       </c>
       <c r="F74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5244745683629475</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <f t="shared" si="5"/>
+        <v>6.2360956446232363</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>7.3</v>
       </c>
@@ -9597,15 +10569,19 @@
         <v>39</v>
       </c>
       <c r="E75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="F75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9160797830996161</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>4.3204937989385739</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>7.4</v>
       </c>
@@ -9619,15 +10595,19 @@
         <v>18</v>
       </c>
       <c r="E76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.666666666666666</v>
       </c>
       <c r="F76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.9581140290126391</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>4.0276819911981905</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>7.5</v>
       </c>
@@ -9641,15 +10621,19 @@
         <v>24</v>
       </c>
       <c r="E77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="F77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.0990195135927845</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <f t="shared" si="5"/>
+        <v>2.1602468994692869</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>7.6</v>
       </c>
@@ -9663,15 +10647,19 @@
         <v>36</v>
       </c>
       <c r="E78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43.666666666666664</v>
       </c>
       <c r="F78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.6080758671996698</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <f t="shared" si="5"/>
+        <v>6.1282587702834119</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>7.7</v>
       </c>
@@ -9685,15 +10673,19 @@
         <v>42</v>
       </c>
       <c r="E79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39.666666666666664</v>
       </c>
       <c r="F79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.2981478758970608</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>2.0548046676563256</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>7.8</v>
       </c>
@@ -9707,15 +10699,19 @@
         <v>25</v>
       </c>
       <c r="E80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.333333333333332</v>
       </c>
       <c r="F80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.41602560309064</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <f t="shared" si="5"/>
+        <v>6.8475461947247123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>7.9</v>
       </c>
@@ -9729,15 +10725,19 @@
         <v>15</v>
       </c>
       <c r="E81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.333333333333332</v>
       </c>
       <c r="F81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.0414518843273806</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <f t="shared" si="5"/>
+        <v>1.247219128924647</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>8</v>
       </c>
@@ -9751,12 +10751,16 @@
         <v>3</v>
       </c>
       <c r="E82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8257418583505538</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="5"/>
+        <v>1.247219128924647</v>
       </c>
     </row>
   </sheetData>
@@ -11779,7 +12783,7 @@
   <dimension ref="A1:A81"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>